<commit_message>
Close #35 - Create DAO's objects
- Created DAO's objects:
	* SupplyDAO
	* ToolDAO
	* BorrowerDAO
	* ToolTypeDAO (should be modified)

- Changed ToolSystem, SupplySystem and BorrowerSystem: i replaced the
populated methods by setList. This setList methods are used in App.java

- Added Tools, Supplies and Borrowers like tables (sheets) in Test.xlsx
</commit_message>
<xml_diff>
--- a/excel/Test.xlsx
+++ b/excel/Test.xlsx
@@ -3,20 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Desktop\Facultad\Proyecto Profesional II\PP2-Project\administrador-herramientas-java\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Pepito" sheetId="1" r:id="rId1"/>
+    <sheet name="Tools" sheetId="1" r:id="rId1"/>
+    <sheet name="Supplies" sheetId="3" r:id="rId2"/>
+    <sheet name="Borrowers" sheetId="4" r:id="rId3"/>
+    <sheet name="ToolTypes" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -32,32 +35,82 @@
     <t>NAME</t>
   </si>
   <si>
-    <t>Chris</t>
-  </si>
-  <si>
-    <t>Cristian</t>
+    <t>Taladro #1</t>
+  </si>
+  <si>
+    <t>Taladro #2</t>
+  </si>
+  <si>
+    <t>Taladro #3</t>
+  </si>
+  <si>
+    <t>Destornillador #1</t>
+  </si>
+  <si>
+    <t>Destornillador #2</t>
+  </si>
+  <si>
+    <t>Destornillador #3</t>
+  </si>
+  <si>
+    <t>Martillo #1</t>
+  </si>
+  <si>
+    <t>Martillo #2</t>
+  </si>
+  <si>
+    <t>Martillo #3</t>
+  </si>
+  <si>
+    <t>IdToolType</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Taladros</t>
+  </si>
+  <si>
+    <t>Destornilladores</t>
+  </si>
+  <si>
+    <t>Martillos</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>MinimumStock</t>
+  </si>
+  <si>
+    <t>Tornillos</t>
+  </si>
+  <si>
+    <t>Clavos</t>
+  </si>
+  <si>
+    <t>Lamparas</t>
+  </si>
+  <si>
+    <t>Tubos de luz</t>
   </si>
   <si>
     <t>Goku</t>
   </si>
   <si>
-    <t>Pluto</t>
-  </si>
-  <si>
-    <t>Mickey</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Prueba</t>
+    <t>Vegeta</t>
+  </si>
+  <si>
+    <t>Gohan</t>
+  </si>
+  <si>
+    <t>Trunks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,8 +146,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -369,20 +450,272 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>80</v>
+      </c>
+      <c r="D3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -390,7 +723,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -398,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -406,43 +739,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7"/>
-      <c r="B7"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Close #38 - Add loans with ExcelDB
- Added the method Add in LoanDAO
- Added a folder with a copy of Test.xlsx in /core folder for gradle
- Added some gets/sets in some entities
- Modify GetLoans method in LoanSystem
- Modify some test class
</commit_message>
<xml_diff>
--- a/excel/Test.xlsx
+++ b/excel/Test.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Desktop\Facultad\Proyecto Profesional II\PP2-Project\administrador-herramientas-java\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView activeTab="3" windowHeight="7620" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tools" sheetId="1" r:id="rId1"/>
-    <sheet name="Supplies" sheetId="3" r:id="rId2"/>
-    <sheet name="Borrowers" sheetId="4" r:id="rId3"/>
-    <sheet name="ToolTypes" sheetId="2" r:id="rId4"/>
+    <sheet name="Tools" r:id="rId1" sheetId="1"/>
+    <sheet name="Supplies" r:id="rId2" sheetId="3"/>
+    <sheet name="Borrowers" r:id="rId3" sheetId="4"/>
+    <sheet name="Loans" r:id="rId4" sheetId="5"/>
+    <sheet name="ToolTypes" r:id="rId5" sheetId="2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -105,14 +106,56 @@
   </si>
   <si>
     <t>Trunks</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>Borrower</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Expiration</t>
+  </si>
+  <si>
+    <t>Tue May 22 16:42:08 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>Wed May 23 16:42:08 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Tue May 22 22:52:24 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>Wed May 23 22:52:24 GMT-03:00 2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -138,13 +181,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -170,10 +215,10 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2">
+    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
+      <tableStyleElement dxfId="1" type="wholeTable"/>
+      <tableStyleElement dxfId="0" type="headerRow"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -192,10 +237,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -230,7 +275,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -265,7 +310,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -359,21 +404,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -390,7 +435,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -442,15 +487,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -569,13 +614,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -652,16 +697,16 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -693,25 +738,127 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -743,6 +890,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Close #40 - Notifications View
- Merge against branch #38
- NotificationsVIew added
- Notification component added
- Conflicts Resolutions added
</commit_message>
<xml_diff>
--- a/excel/Test.xlsx
+++ b/excel/Test.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Desktop\Facultad\Proyecto Profesional II\PP2-Project\administrador-herramientas-java\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView activeTab="3" windowHeight="7620" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tools" sheetId="1" r:id="rId1"/>
-    <sheet name="Supplies" sheetId="3" r:id="rId2"/>
-    <sheet name="Borrowers" sheetId="4" r:id="rId3"/>
-    <sheet name="ToolTypes" sheetId="2" r:id="rId4"/>
+    <sheet name="Tools" r:id="rId1" sheetId="1"/>
+    <sheet name="Supplies" r:id="rId2" sheetId="3"/>
+    <sheet name="Borrowers" r:id="rId3" sheetId="4"/>
+    <sheet name="Loans" r:id="rId4" sheetId="5"/>
+    <sheet name="ToolTypes" r:id="rId5" sheetId="2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -105,14 +106,56 @@
   </si>
   <si>
     <t>Trunks</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>Borrower</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Expiration</t>
+  </si>
+  <si>
+    <t>Tue May 22 16:42:08 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>Wed May 23 16:42:08 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Tue May 22 22:52:24 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>Wed May 23 22:52:24 GMT-03:00 2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -138,13 +181,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -170,10 +215,10 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2">
+    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
+      <tableStyleElement dxfId="1" type="wholeTable"/>
+      <tableStyleElement dxfId="0" type="headerRow"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -192,10 +237,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -230,7 +275,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -265,7 +310,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -359,21 +404,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -390,7 +435,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -442,15 +487,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -569,13 +614,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -652,16 +697,16 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -693,25 +738,127 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -743,6 +890,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Close #47 - Merge release 23/05
</commit_message>
<xml_diff>
--- a/excel/Test.xlsx
+++ b/excel/Test.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Desktop\Facultad\Proyecto Profesional II\PP2-Project\administrador-herramientas-java\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="7620" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" windowHeight="11595" windowWidth="25755" xWindow="360" yWindow="30"/>
   </bookViews>
   <sheets>
     <sheet name="Tools" r:id="rId1" sheetId="1"/>
@@ -18,17 +13,12 @@
     <sheet name="Loans" r:id="rId4" sheetId="5"/>
     <sheet name="ToolTypes" r:id="rId5" sheetId="2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -166,63 +156,574 @@
   </si>
   <si>
     <t>Thu May 24 16:12:42 GMT-03:00 2018</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Wed May 23 16:49:17 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 24 16:49:17 ART 2018</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Wed May 23 16:53:41 ART 2018</t>
+  </si>
+  <si>
+    <t>Thu May 24 16:53:41 ART 2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
+  <fonts count="21">
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="10"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFF0000"/>
+    </font>
+    <font>
+      <sz val="18.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF3F3F76"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF3F3F3F"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFA7D00"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFA7D00"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF006100"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF9C0006"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF9C6500"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="0"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF7F7F7F"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599990"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599990"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599990"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599990"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599990"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799980"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599990"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399980"/>
+      </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <bottom style="thick">
+        <color rgb="FFACCCEA"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <bottom style="medium">
+        <color theme="4" tint="0.399980"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
+    </border>
+    <border>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="7"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="41"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="5"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="2" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="6" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="7" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="3" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="4" fontId="10" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="4" fontId="11" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="5" fontId="12" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="0" fontId="13" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="14" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="15" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="16" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="19" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="19" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="20" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="29"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="33"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="37"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="41"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="45"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="26"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="30"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="34"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="38"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="42"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="46"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="27"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="31"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="35"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="39"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="43"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="47"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="24"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="28"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="32"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="36"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="40"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="44"/>
+    <cellStyle builtinId="27" name="Bad" xfId="22"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="17"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="18"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="2"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="5"/>
+    <cellStyle builtinId="53" name="Explanatory Text" xfId="48"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="7"/>
+    <cellStyle builtinId="26" name="Good" xfId="21"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="11"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="12"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="13"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="14"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="6"/>
+    <cellStyle builtinId="20" name="Input" xfId="15"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="19"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="23"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="10" name="Note" xfId="8"/>
+    <cellStyle builtinId="21" name="Output" xfId="16"/>
+    <cellStyle builtinId="5" name="Percent" xfId="3"/>
+    <cellStyle builtinId="15" name="Title" xfId="10"/>
+    <cellStyle builtinId="25" name="Total" xfId="20"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="9"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
+        <color rgb="FF000000"/>
       </font>
       <fill>
         <patternFill>
@@ -232,30 +733,21 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <color rgb="FF000000"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2">
-    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
+    <tableStyle count="2" name="MySqlDefault" pivot="0">
       <tableStyleElement dxfId="1" type="wholeTable"/>
       <tableStyleElement dxfId="0" type="headerRow"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -521,454 +1013,505 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.000000"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="9.00500011" outlineLevel="0" collapsed="false"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row ht="16.500000" r="1" spans="1:4">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row ht="16.500000" r="2" spans="1:4">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="D2" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row ht="16.500000" r="3" spans="1:4">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="D3" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row ht="16.500000" r="4" spans="1:4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="D4" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row ht="16.500000" r="5" spans="1:4">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="D5" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row ht="16.500000" r="6" spans="1:4">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="D6" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row ht="16.500000" r="7" spans="1:4">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C7">
+      <c r="D7" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:4"/>
+    <row ht="16.500000" r="9" spans="1:4">
+      <c r="A9" s="0">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
+      <c r="D9" s="0">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row ht="16.500000" r="10" spans="1:4">
+      <c r="A10" s="0">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C10" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C9">
+      <c r="D10" s="0">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
+    <row ht="16.500000" r="11" spans="1:4">
+      <c r="A11" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C10">
+      <c r="D11" s="0">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.000000"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:4">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>100</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:4">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>80</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>50</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:4">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <v>20</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.000000"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1">
+      <c r="A2" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:1">
+      <c r="A3" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" s="0" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" s="0" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultRowHeight="15.000000"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.37999916" outlineLevel="0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="33.88000107" outlineLevel="0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="33.13000107" outlineLevel="0" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row ht="16.500000" r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row ht="16.500000" r="2" spans="1:5">
+      <c r="A2" s="0">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row ht="16.500000" r="3" spans="1:5">
+      <c r="A3" s="0">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row ht="16.500000" r="4" spans="1:5">
+      <c r="A4" s="0">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
+    <row ht="16.500000" r="5" spans="1:5">
+      <c r="A5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="0" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s">
+    <row ht="16.500000" r="6" spans="1:5">
+      <c r="A6" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="0" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
+    <row ht="16.500000" r="7" spans="1:5">
+      <c r="A7" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="0" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s">
+    <row ht="16.500000" r="8" spans="1:5">
+      <c r="A8" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="0" t="s">
         <v>45</v>
       </c>
     </row>
+    <row ht="16.500000" r="9" spans="1:5">
+      <c r="A9" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.000000"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.13000011" outlineLevel="0" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:2">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:2">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.30" header="0.30" left="0.70" right="0.70" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>